<commit_message>
Added new parsing variables
</commit_message>
<xml_diff>
--- a/yw_react_fe/yw-fe/testFiles/yw_reference_tables_bad.xlsx
+++ b/yw_react_fe/yw-fe/testFiles/yw_reference_tables_bad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/dev/YW-sludge-modelling-app/yw_react_fe/yw-fe/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0616A872-0909-5A4D-8A7B-F38E82DD68BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB24221-94BD-CE49-8CFC-46E1B9D266B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20600" yWindow="1640" windowWidth="29040" windowHeight="15840" xr2:uid="{455B0008-4095-42C4-8FA9-2EDAC3BC0A90}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="59">
   <si>
     <t>HAWES/STW</t>
   </si>
@@ -573,7 +573,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -782,9 +782,6 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
       <c r="B11">
         <v>10</v>
       </c>

</xml_diff>